<commit_message>
Completed TOOLB, SAVD, LALL, & SALL Feature ID's
</commit_message>
<xml_diff>
--- a/P07/Scrum.xlsx
+++ b/P07/Scrum.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="200">
   <si>
     <t xml:space="preserve">Product Name:</t>
   </si>
@@ -196,6 +196,9 @@
     <t xml:space="preserve">LOGO</t>
   </si>
   <si>
+    <t xml:space="preserve">In Work</t>
+  </si>
+  <si>
     <t xml:space="preserve">Customer</t>
   </si>
   <si>
@@ -209,6 +212,9 @@
   </si>
   <si>
     <t xml:space="preserve">TOOLB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finished in Sprint 3</t>
   </si>
   <si>
     <t xml:space="preserve">Add a toolbar to the user interface</t>
@@ -598,9 +604,6 @@
     <t xml:space="preserve">MixIn Class created. Debugging toString Method for multiple MixIns.</t>
   </si>
   <si>
-    <t xml:space="preserve">In Work</t>
-  </si>
-  <si>
     <t xml:space="preserve">Scoop Class created. Debugging toString Method for multiple MixIns.</t>
   </si>
   <si>
@@ -614,6 +617,24 @@
   </si>
   <si>
     <t xml:space="preserve">Completed Day 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added Toolbar with customized icons. Need to reformat to same size.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Completed Day 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added Save function allowing user to save to a default file.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added Load function allowing user to open a specified file.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added SaveAs function allowing user to save a specified file.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In production.</t>
   </si>
   <si>
     <t xml:space="preserve">--&gt; Add tasks to complete each feature for this sprint</t>
@@ -1042,7 +1063,649 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Product Backlog Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0822559490350384"/>
+          <c:y val="0.161937192584185"/>
+          <c:w val="0.884142152270314"/>
+          <c:h val="0.635515197376718"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="line"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Product Backlog'!$A$12:$A$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Product Backlog'!$B$12:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="61608520"/>
+        <c:axId val="80551593"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="61608520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="6"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Sprints</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="80551593"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="80551593"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Features Remaining at end of Sprint</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="61608520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Sprint Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 01 Backlog'!$B$7:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="0"/>
+        <c:axId val="23589955"/>
+        <c:axId val="53162313"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="23589955"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Days</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="53162313"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="53162313"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="23589955"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1170,11 +1833,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="82070009"/>
-        <c:axId val="39381815"/>
+        <c:axId val="73858213"/>
+        <c:axId val="70016303"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82070009"/>
+        <c:axId val="73858213"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1239,7 +1902,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39381815"/>
+        <c:crossAx val="70016303"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1247,7 +1910,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39381815"/>
+        <c:axId val="70016303"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1321,7 +1984,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82070009"/>
+        <c:crossAx val="73858213"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1348,7 +2011,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1440,25 +2103,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1</c:v>
@@ -1476,11 +2139,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="1223936"/>
-        <c:axId val="19557365"/>
+        <c:axId val="82296128"/>
+        <c:axId val="9504808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1223936"/>
+        <c:axId val="82296128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1545,7 +2208,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19557365"/>
+        <c:crossAx val="9504808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1553,7 +2216,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="19557365"/>
+        <c:axId val="9504808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1627,7 +2290,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1223936"/>
+        <c:crossAx val="82296128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1654,7 +2317,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1782,11 +2445,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="30384123"/>
-        <c:axId val="28231488"/>
+        <c:axId val="70546418"/>
+        <c:axId val="2989364"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="30384123"/>
+        <c:axId val="70546418"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1851,7 +2514,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28231488"/>
+        <c:crossAx val="2989364"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1859,7 +2522,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="28231488"/>
+        <c:axId val="2989364"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1933,7 +2596,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30384123"/>
+        <c:crossAx val="70546418"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1960,7 +2623,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2088,11 +2751,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="57479448"/>
-        <c:axId val="75188556"/>
+        <c:axId val="99978044"/>
+        <c:axId val="64797761"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="57479448"/>
+        <c:axId val="99978044"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2157,7 +2820,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75188556"/>
+        <c:crossAx val="64797761"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2165,7 +2828,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75188556"/>
+        <c:axId val="64797761"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2239,7 +2902,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57479448"/>
+        <c:crossAx val="99978044"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2266,7 +2929,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2394,11 +3057,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="56930722"/>
-        <c:axId val="54492245"/>
+        <c:axId val="33905607"/>
+        <c:axId val="75757744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="56930722"/>
+        <c:axId val="33905607"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2463,7 +3126,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54492245"/>
+        <c:crossAx val="75757744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2471,7 +3134,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="54492245"/>
+        <c:axId val="75757744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2545,649 +3208,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56930722"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Product Backlog Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.0822508118910817"/>
-          <c:y val="0.161916771752837"/>
-          <c:w val="0.884211841119161"/>
-          <c:h val="0.635561160151324"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:scatterChart>
-        <c:scatterStyle val="line"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Product Backlog'!$A$12:$A$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Product Backlog'!$B$12:$B$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>34</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:axId val="22285251"/>
-        <c:axId val="83672641"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="22285251"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="6"/>
-          <c:min val="0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Sprints</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="83672641"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="83672641"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" lang="en-US" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Features Remaining at end of Sprint</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="22285251"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="span"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Sprint Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint 01 Backlog'!$B$7:$B$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="0"/>
-        <c:axId val="78894122"/>
-        <c:axId val="61925446"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="78894122"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Days</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="61925446"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="61925446"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Tasks</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="78894122"/>
+        <c:crossAx val="33905607"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3225,9 +3246,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>3201480</xdr:colOff>
+      <xdr:colOff>3201120</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>119880</xdr:rowOff>
+      <xdr:rowOff>119520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3235,8 +3256,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9115560" y="268200"/>
-        <a:ext cx="5763960" cy="2854440"/>
+        <a:off x="9114840" y="268200"/>
+        <a:ext cx="5763600" cy="2854080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3260,9 +3281,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>517680</xdr:colOff>
+      <xdr:colOff>517320</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>128880</xdr:rowOff>
+      <xdr:rowOff>128520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3270,8 +3291,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4092120" y="446400"/>
-        <a:ext cx="3746880" cy="1847160"/>
+        <a:off x="4093200" y="446400"/>
+        <a:ext cx="3746880" cy="1846800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3295,9 +3316,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>517680</xdr:colOff>
+      <xdr:colOff>517320</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>128880</xdr:rowOff>
+      <xdr:rowOff>128520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3305,8 +3326,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4092120" y="446400"/>
-        <a:ext cx="3746880" cy="1847160"/>
+        <a:off x="4093200" y="446400"/>
+        <a:ext cx="3746880" cy="1846800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3330,9 +3351,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>517680</xdr:colOff>
+      <xdr:colOff>517320</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>128880</xdr:rowOff>
+      <xdr:rowOff>128520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3340,8 +3361,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4092120" y="446400"/>
-        <a:ext cx="3746880" cy="1847160"/>
+        <a:off x="4093200" y="446400"/>
+        <a:ext cx="3746880" cy="1846800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3365,9 +3386,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>517680</xdr:colOff>
+      <xdr:colOff>517320</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>128880</xdr:rowOff>
+      <xdr:rowOff>128520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3375,8 +3396,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4092120" y="446400"/>
-        <a:ext cx="3746880" cy="1847160"/>
+        <a:off x="4093200" y="446400"/>
+        <a:ext cx="3746880" cy="1846800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3400,9 +3421,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>517680</xdr:colOff>
+      <xdr:colOff>517320</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>128880</xdr:rowOff>
+      <xdr:rowOff>128520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3410,8 +3431,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4092120" y="446400"/>
-        <a:ext cx="3746880" cy="1847160"/>
+        <a:off x="4093200" y="446400"/>
+        <a:ext cx="3746880" cy="1846800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3435,9 +3456,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>517680</xdr:colOff>
+      <xdr:colOff>517320</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>128880</xdr:rowOff>
+      <xdr:rowOff>128520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3445,8 +3466,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4092120" y="446400"/>
-        <a:ext cx="3746880" cy="1847160"/>
+        <a:off x="4093200" y="446400"/>
+        <a:ext cx="3746880" cy="1846800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3468,7 +3489,7 @@
   <dimension ref="A1:K102"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3672,11 +3693,11 @@
       </c>
       <c r="B15" s="3" t="n">
         <f aca="false">B14-C15</f>
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C15" s="10" t="n">
         <f aca="false">COUNTIF(G$24:G$108,"Finished in Sprint 3")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="3"/>
@@ -3696,7 +3717,7 @@
       </c>
       <c r="B16" s="3" t="n">
         <f aca="false">B15-C16</f>
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C16" s="10" t="n">
         <f aca="false">COUNTIF(G$24:G$108,"Finished in Sprint 4")</f>
@@ -3716,7 +3737,7 @@
       </c>
       <c r="B17" s="3" t="n">
         <f aca="false">B16-C17</f>
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C17" s="10" t="n">
         <f aca="false">COUNTIF(G$24:G$108,"Finished in Sprint 5")</f>
@@ -3736,7 +3757,7 @@
       </c>
       <c r="B18" s="3" t="n">
         <f aca="false">B17-C18</f>
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C18" s="10" t="n">
         <f aca="false">COUNTIF(G$24:G$108,"Finished in Sprint 6")</f>
@@ -4051,24 +4072,28 @@
       <c r="E30" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="F30" s="17"/>
-      <c r="G30" s="18"/>
+      <c r="F30" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="G30" s="18" t="s">
+        <v>56</v>
+      </c>
       <c r="H30" s="14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I30" s="19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J30" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K30" s="19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B31" s="11" t="n">
         <v>8</v>
@@ -4080,24 +4105,28 @@
       <c r="E31" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="F31" s="17"/>
-      <c r="G31" s="18"/>
+      <c r="F31" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="G31" s="18" t="s">
+        <v>62</v>
+      </c>
       <c r="H31" s="14" t="s">
         <v>32</v>
       </c>
       <c r="I31" s="19" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="J31" s="19" t="s">
         <v>50</v>
       </c>
       <c r="K31" s="19" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B32" s="11" t="n">
         <v>9</v>
@@ -4109,22 +4138,26 @@
       <c r="E32" s="11" t="n">
         <v>8</v>
       </c>
-      <c r="F32" s="17"/>
-      <c r="G32" s="18"/>
+      <c r="F32" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="G32" s="18" t="s">
+        <v>62</v>
+      </c>
       <c r="H32" s="14" t="s">
         <v>32</v>
       </c>
       <c r="I32" s="19" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J32" s="19" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="K32" s="19"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B33" s="11" t="n">
         <v>10</v>
@@ -4136,22 +4169,26 @@
       <c r="E33" s="11" t="n">
         <v>8</v>
       </c>
-      <c r="F33" s="17"/>
-      <c r="G33" s="18"/>
+      <c r="F33" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="G33" s="18" t="s">
+        <v>62</v>
+      </c>
       <c r="H33" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I33" s="19" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="J33" s="19" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="K33" s="19"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B34" s="11" t="n">
         <v>11</v>
@@ -4163,22 +4200,26 @@
       <c r="E34" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="F34" s="17"/>
-      <c r="G34" s="18"/>
+      <c r="F34" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="G34" s="18" t="s">
+        <v>62</v>
+      </c>
       <c r="H34" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I34" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="J34" s="19" t="s">
         <v>71</v>
-      </c>
-      <c r="J34" s="19" t="s">
-        <v>69</v>
       </c>
       <c r="K34" s="19"/>
     </row>
     <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B35" s="11" t="n">
         <v>12</v>
@@ -4196,18 +4237,18 @@
         <v>32</v>
       </c>
       <c r="I35" s="19" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J35" s="19" t="s">
         <v>34</v>
       </c>
       <c r="K35" s="19" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B36" s="11" t="n">
         <v>13</v>
@@ -4222,21 +4263,21 @@
       <c r="F36" s="17"/>
       <c r="G36" s="18"/>
       <c r="H36" s="14" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I36" s="19" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="J36" s="19" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K36" s="19" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B37" s="11" t="n">
         <v>14</v>
@@ -4254,16 +4295,16 @@
         <v>32</v>
       </c>
       <c r="I37" s="19" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="J37" s="19" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K37" s="19"/>
     </row>
     <row r="38" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B38" s="11" t="n">
         <v>15</v>
@@ -4278,19 +4319,19 @@
       <c r="F38" s="17"/>
       <c r="G38" s="18"/>
       <c r="H38" s="14" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I38" s="19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="J38" s="19" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="K38" s="19"/>
     </row>
     <row r="39" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B39" s="11" t="n">
         <v>16</v>
@@ -4305,19 +4346,19 @@
       <c r="F39" s="17"/>
       <c r="G39" s="18"/>
       <c r="H39" s="14" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I39" s="19" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="J39" s="19" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K39" s="19"/>
     </row>
     <row r="40" s="20" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B40" s="11" t="n">
         <v>17</v>
@@ -4332,21 +4373,21 @@
       <c r="F40" s="17"/>
       <c r="G40" s="18"/>
       <c r="H40" s="14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I40" s="19" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="J40" s="19" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="K40" s="19" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B41" s="11" t="n">
         <v>18</v>
@@ -4361,21 +4402,21 @@
       <c r="F41" s="17"/>
       <c r="G41" s="18"/>
       <c r="H41" s="14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I41" s="19" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="J41" s="19" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="K41" s="19" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" s="20" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B42" s="11" t="n">
         <v>19</v>
@@ -4393,18 +4434,18 @@
         <v>32</v>
       </c>
       <c r="I42" s="19" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="J42" s="19" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="K42" s="19" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" s="20" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B43" s="11" t="n">
         <v>20</v>
@@ -4422,16 +4463,16 @@
         <v>32</v>
       </c>
       <c r="I43" s="19" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J43" s="19" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K43" s="19"/>
     </row>
     <row r="44" s="20" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B44" s="11" t="n">
         <v>21</v>
@@ -4446,21 +4487,21 @@
       <c r="F44" s="17"/>
       <c r="G44" s="18"/>
       <c r="H44" s="14" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I44" s="19" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="J44" s="19" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="K44" s="19" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="45" s="20" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B45" s="11" t="n">
         <v>22</v>
@@ -4475,21 +4516,21 @@
       <c r="F45" s="17"/>
       <c r="G45" s="18"/>
       <c r="H45" s="14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I45" s="19" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="J45" s="19" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="K45" s="19" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B46" s="11" t="n">
         <v>23</v>
@@ -4504,21 +4545,21 @@
       <c r="F46" s="17"/>
       <c r="G46" s="18"/>
       <c r="H46" s="14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I46" s="19" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="J46" s="19" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="K46" s="19" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B47" s="11" t="n">
         <v>24</v>
@@ -4531,19 +4572,19 @@
       <c r="F47" s="17"/>
       <c r="G47" s="18"/>
       <c r="H47" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I47" s="19" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="J47" s="19" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="K47" s="19"/>
     </row>
     <row r="48" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B48" s="11" t="n">
         <v>25</v>
@@ -4556,19 +4597,19 @@
       <c r="F48" s="17"/>
       <c r="G48" s="18"/>
       <c r="H48" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I48" s="19" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="J48" s="19" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="K48" s="19"/>
     </row>
     <row r="49" s="21" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B49" s="11" t="n">
         <v>26</v>
@@ -4584,16 +4625,16 @@
         <v>32</v>
       </c>
       <c r="I49" s="19" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J49" s="19" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K49" s="19"/>
     </row>
     <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B50" s="11" t="n">
         <v>27</v>
@@ -4609,16 +4650,16 @@
         <v>32</v>
       </c>
       <c r="I50" s="19" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="J50" s="19" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="K50" s="19"/>
     </row>
     <row r="51" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B51" s="11" t="n">
         <v>28</v>
@@ -4634,16 +4675,16 @@
         <v>32</v>
       </c>
       <c r="I51" s="19" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="J51" s="19" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="K51" s="19"/>
     </row>
     <row r="52" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B52" s="11" t="n">
         <v>29</v>
@@ -4659,16 +4700,16 @@
         <v>32</v>
       </c>
       <c r="I52" s="19" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="J52" s="19" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="K52" s="19"/>
     </row>
     <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B53" s="11" t="n">
         <v>30</v>
@@ -4681,19 +4722,19 @@
       <c r="F53" s="17"/>
       <c r="G53" s="18"/>
       <c r="H53" s="14" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I53" s="19" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="J53" s="19" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K53" s="19"/>
     </row>
     <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B54" s="11" t="n">
         <v>31</v>
@@ -4706,21 +4747,21 @@
       <c r="F54" s="17"/>
       <c r="G54" s="18"/>
       <c r="H54" s="14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I54" s="19" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="J54" s="19" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="K54" s="19" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B55" s="11" t="n">
         <v>32</v>
@@ -4736,16 +4777,16 @@
         <v>32</v>
       </c>
       <c r="I55" s="19" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="J55" s="19" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="K55" s="19"/>
     </row>
     <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B56" s="11" t="n">
         <v>33</v>
@@ -4761,16 +4802,16 @@
         <v>32</v>
       </c>
       <c r="I56" s="19" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="J56" s="19" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="K56" s="19"/>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B57" s="11" t="n">
         <v>34</v>
@@ -4786,16 +4827,16 @@
         <v>32</v>
       </c>
       <c r="I57" s="19" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="J57" s="19" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="K57" s="19"/>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B58" s="11" t="n">
         <v>35</v>
@@ -4811,16 +4852,16 @@
         <v>32</v>
       </c>
       <c r="I58" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="J58" s="19" t="s">
         <v>148</v>
-      </c>
-      <c r="J58" s="19" t="s">
-        <v>146</v>
       </c>
       <c r="K58" s="19"/>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B59" s="11" t="n">
         <v>36</v>
@@ -4836,16 +4877,16 @@
         <v>32</v>
       </c>
       <c r="I59" s="19" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="J59" s="19" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="K59" s="19"/>
     </row>
     <row r="60" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B60" s="11" t="n">
         <v>37</v>
@@ -4861,16 +4902,16 @@
         <v>32</v>
       </c>
       <c r="I60" s="19" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="J60" s="19" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="K60" s="19"/>
     </row>
     <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B61" s="11" t="n">
         <v>38</v>
@@ -4886,16 +4927,16 @@
         <v>32</v>
       </c>
       <c r="I61" s="19" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="J61" s="19" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="K61" s="19"/>
     </row>
     <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B62" s="11" t="n">
         <v>39</v>
@@ -4911,16 +4952,16 @@
         <v>32</v>
       </c>
       <c r="I62" s="19" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="J62" s="19" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="K62" s="19"/>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B63" s="11" t="n">
         <v>40</v>
@@ -4936,10 +4977,10 @@
         <v>32</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="J63" s="19" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="K63" s="19"/>
     </row>
@@ -5443,7 +5484,7 @@
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -5467,21 +5508,21 @@
     </row>
     <row r="2" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B2" s="25" t="n">
         <v>44831</v>
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="26" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
     </row>
     <row r="3" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B3" s="25" t="n">
         <v>44838</v>
@@ -5493,10 +5534,10 @@
     </row>
     <row r="4" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
@@ -5517,7 +5558,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -5525,7 +5566,7 @@
     </row>
     <row r="7" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B7" s="22" t="n">
         <v>4</v>
@@ -5537,7 +5578,7 @@
     </row>
     <row r="8" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B8" s="22" t="n">
         <f aca="false">B7-C8</f>
@@ -5553,7 +5594,7 @@
     </row>
     <row r="9" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B9" s="22" t="n">
         <f aca="false">B8-C9</f>
@@ -5569,7 +5610,7 @@
     </row>
     <row r="10" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B10" s="22" t="n">
         <f aca="false">B9-C10</f>
@@ -5585,7 +5626,7 @@
     </row>
     <row r="11" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B11" s="22" t="n">
         <f aca="false">B10-C11</f>
@@ -5601,7 +5642,7 @@
     </row>
     <row r="12" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B12" s="22" t="n">
         <f aca="false">B11-C12</f>
@@ -5617,7 +5658,7 @@
     </row>
     <row r="13" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B13" s="22" t="n">
         <f aca="false">B12-C13</f>
@@ -5633,7 +5674,7 @@
     </row>
     <row r="14" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B14" s="22" t="n">
         <f aca="false">B13-C14</f>
@@ -5657,16 +5698,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B16" s="29" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E16" s="29" t="s">
         <v>25</v>
@@ -5683,10 +5724,10 @@
         <v>30</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5697,10 +5738,10 @@
         <v>36</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5711,10 +5752,10 @@
         <v>39</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E19" s="32" t="s">
-        <v>184</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5725,10 +5766,10 @@
         <v>43</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E20" s="32" t="s">
-        <v>184</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5739,10 +5780,10 @@
         <v>39</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E21" s="32" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5753,10 +5794,10 @@
         <v>43</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E22" s="32" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6432,11 +6473,11 @@
   </sheetPr>
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -6461,7 +6502,7 @@
     </row>
     <row r="2" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B2" s="25" t="n">
         <f aca="false">'Sprint 01 Backlog'!B3</f>
@@ -6469,14 +6510,14 @@
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="26" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
     </row>
     <row r="3" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B3" s="25" t="n">
         <f aca="false">B2+7</f>
@@ -6489,10 +6530,10 @@
     </row>
     <row r="4" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
@@ -6513,7 +6554,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -6521,7 +6562,7 @@
     </row>
     <row r="7" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B7" s="22" t="n">
         <v>2</v>
@@ -6533,7 +6574,7 @@
     </row>
     <row r="8" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B8" s="22" t="n">
         <f aca="false">B7-C8</f>
@@ -6549,7 +6590,7 @@
     </row>
     <row r="9" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B9" s="22" t="n">
         <f aca="false">B8-C9</f>
@@ -6565,7 +6606,7 @@
     </row>
     <row r="10" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B10" s="22" t="n">
         <f aca="false">B9-C10</f>
@@ -6581,7 +6622,7 @@
     </row>
     <row r="11" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B11" s="22" t="n">
         <f aca="false">B10-C11</f>
@@ -6597,7 +6638,7 @@
     </row>
     <row r="12" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B12" s="22" t="n">
         <f aca="false">B11-C12</f>
@@ -6613,7 +6654,7 @@
     </row>
     <row r="13" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B13" s="22" t="n">
         <f aca="false">B12-C13</f>
@@ -6628,7 +6669,7 @@
     </row>
     <row r="14" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B14" s="22" t="n">
         <f aca="false">B13-C14</f>
@@ -6652,16 +6693,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B16" s="29" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E16" s="29" t="s">
         <v>25</v>
@@ -6678,10 +6719,10 @@
         <v>47</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6692,10 +6733,10 @@
         <v>52</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7399,11 +7440,11 @@
   </sheetPr>
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -7428,7 +7469,7 @@
     </row>
     <row r="2" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B2" s="25" t="n">
         <f aca="false">'Sprint 02 Backlog'!B3</f>
@@ -7436,14 +7477,14 @@
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="26" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
     </row>
     <row r="3" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B3" s="25" t="n">
         <f aca="false">B2+7</f>
@@ -7456,10 +7497,10 @@
     </row>
     <row r="4" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
@@ -7480,7 +7521,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -7488,11 +7529,10 @@
     </row>
     <row r="7" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B7" s="22" t="n">
-        <f aca="false">COUNTA(D17:D995)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
@@ -7501,11 +7541,11 @@
     </row>
     <row r="8" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B8" s="22" t="n">
         <f aca="false">B7-C8</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C8" s="22" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -7517,11 +7557,11 @@
     </row>
     <row r="9" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B9" s="22" t="n">
         <f aca="false">B8-C9</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C9" s="22" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -7533,11 +7573,11 @@
     </row>
     <row r="10" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B10" s="22" t="n">
         <f aca="false">B9-C10</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C10" s="22" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -7549,11 +7589,11 @@
     </row>
     <row r="11" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B11" s="22" t="n">
         <f aca="false">B10-C11</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C11" s="22" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -7565,15 +7605,14 @@
     </row>
     <row r="12" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B12" s="22" t="n">
         <f aca="false">B11-C12</f>
+        <v>4</v>
+      </c>
+      <c r="C12" s="22" t="n">
         <v>1</v>
-      </c>
-      <c r="C12" s="22" t="n">
-        <f aca="false">COUNTIF(E$17:E$995, "Completed Day 5")</f>
-        <v>0</v>
       </c>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
@@ -7581,11 +7620,11 @@
     </row>
     <row r="13" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B13" s="22" t="n">
         <f aca="false">B12-C13</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C13" s="22" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -7597,15 +7636,14 @@
     </row>
     <row r="14" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B14" s="22" t="n">
         <f aca="false">B13-C14</f>
         <v>1</v>
       </c>
       <c r="C14" s="22" t="n">
-        <f aca="false">COUNTIF(E$17:E$995, "Completed Day 7")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
@@ -7621,16 +7659,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B16" s="29" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E16" s="29" t="s">
         <v>25</v>
@@ -7639,679 +7677,707 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B17" s="33"/>
-      <c r="D17" s="35" t="s">
-        <v>190</v>
-      </c>
-      <c r="E17" s="34"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="E17" s="32" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="34"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="34"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="34"/>
+      <c r="B20" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="E20" s="32" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="34"/>
+      <c r="B21" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="E21" s="32" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="34"/>
+      <c r="B22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="32"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="34"/>
+      <c r="B23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="32"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="34"/>
+      <c r="B24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="32"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="B25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="34"/>
+      <c r="B25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="32"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="B26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="34"/>
+      <c r="B26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="32"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="B27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="34"/>
+      <c r="B27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="32"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="B28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="34"/>
+      <c r="B28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="32"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="B29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="34"/>
+      <c r="B29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="32"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="34"/>
+      <c r="B30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="32"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="34"/>
+      <c r="B31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="32"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="B32" s="33"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="34"/>
+      <c r="B32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="32"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="B33" s="33"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="34"/>
+      <c r="B33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="32"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="B34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="34"/>
+      <c r="B34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="32"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="B35" s="33"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="34"/>
+      <c r="B35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="32"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B36" s="33"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="34"/>
+      <c r="B36" s="30"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="32"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="B37" s="33"/>
-      <c r="D37" s="33"/>
-      <c r="E37" s="34"/>
+      <c r="B37" s="30"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="32"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="B38" s="33"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="34"/>
+      <c r="B38" s="30"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="32"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="B39" s="33"/>
-      <c r="D39" s="33"/>
-      <c r="E39" s="34"/>
+      <c r="B39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="32"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="B40" s="33"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="34"/>
+      <c r="B40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="32"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="B41" s="33"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="34"/>
+      <c r="B41" s="30"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="32"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="B42" s="33"/>
-      <c r="D42" s="33"/>
-      <c r="E42" s="34"/>
+      <c r="B42" s="30"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="32"/>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="B43" s="33"/>
-      <c r="D43" s="33"/>
-      <c r="E43" s="34"/>
+      <c r="B43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="32"/>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="B44" s="33"/>
-      <c r="D44" s="33"/>
-      <c r="E44" s="34"/>
+      <c r="B44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="32"/>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="B45" s="33"/>
-      <c r="D45" s="33"/>
-      <c r="E45" s="34"/>
+      <c r="B45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="32"/>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B46" s="33"/>
-      <c r="D46" s="33"/>
-      <c r="E46" s="34"/>
+      <c r="B46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="32"/>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="B47" s="33"/>
-      <c r="D47" s="33"/>
-      <c r="E47" s="34"/>
+      <c r="B47" s="30"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="32"/>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="B48" s="33"/>
-      <c r="D48" s="33"/>
-      <c r="E48" s="34"/>
+      <c r="B48" s="30"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="32"/>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="B49" s="33"/>
-      <c r="D49" s="33"/>
-      <c r="E49" s="34"/>
+      <c r="B49" s="30"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="32"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="B50" s="33"/>
-      <c r="D50" s="33"/>
-      <c r="E50" s="34"/>
+      <c r="B50" s="30"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="32"/>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="B51" s="33"/>
-      <c r="D51" s="33"/>
-      <c r="E51" s="34"/>
+      <c r="B51" s="30"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="32"/>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="B52" s="33"/>
-      <c r="D52" s="33"/>
-      <c r="E52" s="34"/>
+      <c r="B52" s="30"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="32"/>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="B53" s="33"/>
-      <c r="D53" s="33"/>
-      <c r="E53" s="34"/>
+      <c r="B53" s="30"/>
+      <c r="D53" s="30"/>
+      <c r="E53" s="32"/>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="B54" s="33"/>
-      <c r="D54" s="33"/>
-      <c r="E54" s="34"/>
+      <c r="B54" s="30"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="32"/>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="B55" s="33"/>
-      <c r="D55" s="33"/>
-      <c r="E55" s="34"/>
+      <c r="B55" s="30"/>
+      <c r="D55" s="30"/>
+      <c r="E55" s="32"/>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="B56" s="33"/>
-      <c r="D56" s="33"/>
-      <c r="E56" s="34"/>
+      <c r="B56" s="30"/>
+      <c r="D56" s="30"/>
+      <c r="E56" s="32"/>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="B57" s="33"/>
-      <c r="D57" s="33"/>
-      <c r="E57" s="34"/>
+      <c r="B57" s="30"/>
+      <c r="D57" s="30"/>
+      <c r="E57" s="32"/>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="B58" s="33"/>
-      <c r="D58" s="33"/>
-      <c r="E58" s="34"/>
+      <c r="B58" s="30"/>
+      <c r="D58" s="30"/>
+      <c r="E58" s="32"/>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
         <v>43</v>
       </c>
-      <c r="B59" s="33"/>
-      <c r="D59" s="33"/>
-      <c r="E59" s="34"/>
+      <c r="B59" s="30"/>
+      <c r="D59" s="30"/>
+      <c r="E59" s="32"/>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="B60" s="33"/>
-      <c r="D60" s="33"/>
-      <c r="E60" s="34"/>
+      <c r="B60" s="30"/>
+      <c r="D60" s="30"/>
+      <c r="E60" s="32"/>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="B61" s="33"/>
-      <c r="D61" s="33"/>
-      <c r="E61" s="34"/>
+      <c r="B61" s="30"/>
+      <c r="D61" s="30"/>
+      <c r="E61" s="32"/>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
         <v>46</v>
       </c>
-      <c r="B62" s="33"/>
-      <c r="D62" s="33"/>
-      <c r="E62" s="34"/>
+      <c r="B62" s="30"/>
+      <c r="D62" s="30"/>
+      <c r="E62" s="32"/>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
         <v>47</v>
       </c>
-      <c r="B63" s="33"/>
-      <c r="D63" s="33"/>
-      <c r="E63" s="34"/>
+      <c r="B63" s="30"/>
+      <c r="D63" s="30"/>
+      <c r="E63" s="32"/>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="B64" s="33"/>
-      <c r="D64" s="33"/>
-      <c r="E64" s="34"/>
+      <c r="B64" s="30"/>
+      <c r="D64" s="30"/>
+      <c r="E64" s="32"/>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
         <v>49</v>
       </c>
-      <c r="B65" s="33"/>
-      <c r="D65" s="33"/>
-      <c r="E65" s="34"/>
+      <c r="B65" s="30"/>
+      <c r="D65" s="30"/>
+      <c r="E65" s="32"/>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="B66" s="33"/>
-      <c r="D66" s="33"/>
-      <c r="E66" s="34"/>
+      <c r="B66" s="30"/>
+      <c r="D66" s="30"/>
+      <c r="E66" s="32"/>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
         <v>51</v>
       </c>
-      <c r="B67" s="33"/>
-      <c r="D67" s="33"/>
-      <c r="E67" s="34"/>
+      <c r="B67" s="30"/>
+      <c r="D67" s="30"/>
+      <c r="E67" s="32"/>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
         <v>52</v>
       </c>
-      <c r="B68" s="33"/>
-      <c r="D68" s="33"/>
-      <c r="E68" s="34"/>
+      <c r="B68" s="30"/>
+      <c r="D68" s="30"/>
+      <c r="E68" s="32"/>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
         <v>53</v>
       </c>
-      <c r="B69" s="33"/>
-      <c r="D69" s="33"/>
-      <c r="E69" s="34"/>
+      <c r="B69" s="30"/>
+      <c r="D69" s="30"/>
+      <c r="E69" s="32"/>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
         <v>54</v>
       </c>
-      <c r="B70" s="33"/>
-      <c r="D70" s="33"/>
-      <c r="E70" s="34"/>
+      <c r="B70" s="30"/>
+      <c r="D70" s="30"/>
+      <c r="E70" s="32"/>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="B71" s="33"/>
-      <c r="D71" s="33"/>
-      <c r="E71" s="34"/>
+      <c r="B71" s="30"/>
+      <c r="D71" s="30"/>
+      <c r="E71" s="32"/>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
         <v>56</v>
       </c>
-      <c r="B72" s="33"/>
-      <c r="D72" s="33"/>
-      <c r="E72" s="34"/>
+      <c r="B72" s="30"/>
+      <c r="D72" s="30"/>
+      <c r="E72" s="32"/>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
         <v>57</v>
       </c>
-      <c r="B73" s="33"/>
-      <c r="D73" s="33"/>
-      <c r="E73" s="34"/>
+      <c r="B73" s="30"/>
+      <c r="D73" s="30"/>
+      <c r="E73" s="32"/>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
         <v>58</v>
       </c>
-      <c r="B74" s="33"/>
-      <c r="D74" s="33"/>
-      <c r="E74" s="34"/>
+      <c r="B74" s="30"/>
+      <c r="D74" s="30"/>
+      <c r="E74" s="32"/>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="B75" s="33"/>
-      <c r="D75" s="33"/>
-      <c r="E75" s="34"/>
+      <c r="B75" s="30"/>
+      <c r="D75" s="30"/>
+      <c r="E75" s="32"/>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="B76" s="33"/>
-      <c r="D76" s="33"/>
-      <c r="E76" s="34"/>
+      <c r="B76" s="30"/>
+      <c r="D76" s="30"/>
+      <c r="E76" s="32"/>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
         <v>61</v>
       </c>
-      <c r="B77" s="33"/>
-      <c r="D77" s="33"/>
-      <c r="E77" s="34"/>
+      <c r="B77" s="30"/>
+      <c r="D77" s="30"/>
+      <c r="E77" s="32"/>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
         <v>62</v>
       </c>
-      <c r="B78" s="33"/>
-      <c r="D78" s="33"/>
-      <c r="E78" s="34"/>
+      <c r="B78" s="30"/>
+      <c r="D78" s="30"/>
+      <c r="E78" s="32"/>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="n">
         <v>63</v>
       </c>
-      <c r="B79" s="33"/>
-      <c r="D79" s="33"/>
-      <c r="E79" s="34"/>
+      <c r="B79" s="30"/>
+      <c r="D79" s="30"/>
+      <c r="E79" s="32"/>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
         <v>64</v>
       </c>
-      <c r="B80" s="33"/>
-      <c r="D80" s="33"/>
-      <c r="E80" s="34"/>
+      <c r="B80" s="30"/>
+      <c r="D80" s="30"/>
+      <c r="E80" s="32"/>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="B81" s="33"/>
-      <c r="D81" s="33"/>
-      <c r="E81" s="34"/>
+      <c r="B81" s="30"/>
+      <c r="D81" s="30"/>
+      <c r="E81" s="32"/>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="n">
         <v>66</v>
       </c>
-      <c r="B82" s="33"/>
-      <c r="D82" s="33"/>
-      <c r="E82" s="34"/>
+      <c r="B82" s="30"/>
+      <c r="D82" s="30"/>
+      <c r="E82" s="32"/>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="n">
         <v>67</v>
       </c>
-      <c r="B83" s="33"/>
-      <c r="D83" s="33"/>
-      <c r="E83" s="34"/>
+      <c r="B83" s="30"/>
+      <c r="D83" s="30"/>
+      <c r="E83" s="32"/>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
         <v>68</v>
       </c>
-      <c r="B84" s="33"/>
-      <c r="D84" s="33"/>
-      <c r="E84" s="34"/>
+      <c r="B84" s="30"/>
+      <c r="D84" s="30"/>
+      <c r="E84" s="32"/>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="n">
         <v>69</v>
       </c>
-      <c r="B85" s="33"/>
-      <c r="D85" s="33"/>
-      <c r="E85" s="34"/>
+      <c r="B85" s="30"/>
+      <c r="D85" s="30"/>
+      <c r="E85" s="32"/>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="B86" s="33"/>
-      <c r="D86" s="33"/>
-      <c r="E86" s="34"/>
+      <c r="B86" s="30"/>
+      <c r="D86" s="30"/>
+      <c r="E86" s="32"/>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="B87" s="33"/>
-      <c r="D87" s="33"/>
-      <c r="E87" s="34"/>
+      <c r="B87" s="30"/>
+      <c r="D87" s="30"/>
+      <c r="E87" s="32"/>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="n">
         <v>72</v>
       </c>
-      <c r="B88" s="33"/>
-      <c r="D88" s="33"/>
-      <c r="E88" s="34"/>
+      <c r="B88" s="30"/>
+      <c r="D88" s="30"/>
+      <c r="E88" s="32"/>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="n">
         <v>73</v>
       </c>
-      <c r="B89" s="33"/>
-      <c r="D89" s="33"/>
-      <c r="E89" s="34"/>
+      <c r="B89" s="30"/>
+      <c r="D89" s="30"/>
+      <c r="E89" s="32"/>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="n">
         <v>74</v>
       </c>
-      <c r="B90" s="33"/>
-      <c r="D90" s="33"/>
-      <c r="E90" s="34"/>
+      <c r="B90" s="30"/>
+      <c r="D90" s="30"/>
+      <c r="E90" s="32"/>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="n">
         <v>75</v>
       </c>
-      <c r="B91" s="33"/>
-      <c r="D91" s="33"/>
-      <c r="E91" s="34"/>
+      <c r="B91" s="30"/>
+      <c r="D91" s="30"/>
+      <c r="E91" s="32"/>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="n">
         <v>76</v>
       </c>
-      <c r="B92" s="33"/>
-      <c r="D92" s="33"/>
-      <c r="E92" s="34"/>
+      <c r="B92" s="30"/>
+      <c r="D92" s="30"/>
+      <c r="E92" s="32"/>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="n">
         <v>77</v>
       </c>
-      <c r="B93" s="33"/>
-      <c r="D93" s="33"/>
-      <c r="E93" s="34"/>
+      <c r="B93" s="30"/>
+      <c r="D93" s="30"/>
+      <c r="E93" s="32"/>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="n">
         <v>78</v>
       </c>
-      <c r="B94" s="33"/>
-      <c r="D94" s="33"/>
-      <c r="E94" s="34"/>
+      <c r="B94" s="30"/>
+      <c r="D94" s="30"/>
+      <c r="E94" s="32"/>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="n">
         <v>79</v>
       </c>
-      <c r="B95" s="33"/>
-      <c r="D95" s="33"/>
-      <c r="E95" s="34"/>
+      <c r="B95" s="30"/>
+      <c r="D95" s="30"/>
+      <c r="E95" s="32"/>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="B96" s="33"/>
-      <c r="D96" s="33"/>
-      <c r="E96" s="34"/>
+      <c r="B96" s="30"/>
+      <c r="D96" s="30"/>
+      <c r="E96" s="32"/>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="n">
         <v>81</v>
       </c>
-      <c r="B97" s="33"/>
-      <c r="D97" s="33"/>
-      <c r="E97" s="34"/>
+      <c r="B97" s="30"/>
+      <c r="D97" s="30"/>
+      <c r="E97" s="32"/>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="n">
         <v>82</v>
       </c>
-      <c r="B98" s="33"/>
-      <c r="D98" s="33"/>
-      <c r="E98" s="34"/>
+      <c r="B98" s="30"/>
+      <c r="D98" s="30"/>
+      <c r="E98" s="32"/>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="n">
         <v>83</v>
       </c>
-      <c r="B99" s="33"/>
-      <c r="D99" s="33"/>
-      <c r="E99" s="34"/>
+      <c r="B99" s="30"/>
+      <c r="D99" s="30"/>
+      <c r="E99" s="32"/>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="n">
         <v>84</v>
       </c>
-      <c r="B100" s="33"/>
-      <c r="D100" s="33"/>
-      <c r="E100" s="34"/>
+      <c r="B100" s="30"/>
+      <c r="D100" s="30"/>
+      <c r="E100" s="32"/>
     </row>
   </sheetData>
   <dataValidations count="6">
@@ -8327,7 +8393,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature.&#10;&#10;Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the m" promptTitle="Task Description" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D18:D100" type="none">
+    <dataValidation allowBlank="true" operator="equal" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature.&#10;&#10;Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the m" promptTitle="Task Description" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D17:D100" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -8362,7 +8428,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -8387,21 +8453,21 @@
     </row>
     <row r="2" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B2" s="25" t="n">
         <v>44873</v>
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="26" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
     </row>
     <row r="3" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B3" s="25" t="n">
         <f aca="false">B2+7</f>
@@ -8414,10 +8480,10 @@
     </row>
     <row r="4" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
@@ -8438,7 +8504,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -8446,7 +8512,7 @@
     </row>
     <row r="7" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B7" s="22" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
@@ -8459,7 +8525,7 @@
     </row>
     <row r="8" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B8" s="22" t="n">
         <f aca="false">B7-C8</f>
@@ -8475,7 +8541,7 @@
     </row>
     <row r="9" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B9" s="22" t="n">
         <f aca="false">B8-C9</f>
@@ -8491,7 +8557,7 @@
     </row>
     <row r="10" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B10" s="22" t="n">
         <f aca="false">B9-C10</f>
@@ -8507,7 +8573,7 @@
     </row>
     <row r="11" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B11" s="22" t="n">
         <f aca="false">B10-C11</f>
@@ -8523,7 +8589,7 @@
     </row>
     <row r="12" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B12" s="22" t="n">
         <f aca="false">B11-C12</f>
@@ -8539,7 +8605,7 @@
     </row>
     <row r="13" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B13" s="22" t="n">
         <f aca="false">B12-C13</f>
@@ -8555,7 +8621,7 @@
     </row>
     <row r="14" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B14" s="22" t="n">
         <f aca="false">B13-C14</f>
@@ -8579,16 +8645,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B16" s="29" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E16" s="29" t="s">
         <v>25</v>
@@ -8603,7 +8669,7 @@
       </c>
       <c r="B17" s="33"/>
       <c r="D17" s="35" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="E17" s="34"/>
     </row>
@@ -9320,7 +9386,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -9345,7 +9411,7 @@
     </row>
     <row r="2" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B2" s="25" t="n">
         <f aca="false">'Sprint 04 Backlog'!B3</f>
@@ -9353,14 +9419,14 @@
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="26" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
     </row>
     <row r="3" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B3" s="25" t="n">
         <f aca="false">B2+7</f>
@@ -9373,10 +9439,10 @@
     </row>
     <row r="4" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
@@ -9397,7 +9463,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -9405,7 +9471,7 @@
     </row>
     <row r="7" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B7" s="22" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
@@ -9418,7 +9484,7 @@
     </row>
     <row r="8" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B8" s="22" t="n">
         <f aca="false">B7-C8</f>
@@ -9434,7 +9500,7 @@
     </row>
     <row r="9" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B9" s="22" t="n">
         <f aca="false">B8-C9</f>
@@ -9450,7 +9516,7 @@
     </row>
     <row r="10" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B10" s="22" t="n">
         <f aca="false">B9-C10</f>
@@ -9466,7 +9532,7 @@
     </row>
     <row r="11" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B11" s="22" t="n">
         <f aca="false">B10-C11</f>
@@ -9482,7 +9548,7 @@
     </row>
     <row r="12" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B12" s="22" t="n">
         <f aca="false">B11-C12</f>
@@ -9498,7 +9564,7 @@
     </row>
     <row r="13" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B13" s="22" t="n">
         <f aca="false">B12-C13</f>
@@ -9514,7 +9580,7 @@
     </row>
     <row r="14" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B14" s="22" t="n">
         <f aca="false">B13-C14</f>
@@ -9538,16 +9604,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B16" s="29" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E16" s="29" t="s">
         <v>25</v>
@@ -9562,7 +9628,7 @@
       </c>
       <c r="B17" s="33"/>
       <c r="D17" s="35" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="E17" s="34"/>
     </row>
@@ -10279,7 +10345,7 @@
       <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -10296,7 +10362,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="D1" s="23" t="s">
         <v>2</v>
@@ -10305,21 +10371,21 @@
     </row>
     <row r="2" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B2" s="25" t="n">
         <v>44894</v>
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="26" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
     </row>
     <row r="3" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B3" s="25" t="n">
         <f aca="false">B2+7</f>
@@ -10332,10 +10398,10 @@
     </row>
     <row r="4" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
@@ -10356,7 +10422,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -10364,7 +10430,7 @@
     </row>
     <row r="7" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B7" s="22" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
@@ -10377,7 +10443,7 @@
     </row>
     <row r="8" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B8" s="22" t="n">
         <f aca="false">B7-C8</f>
@@ -10393,7 +10459,7 @@
     </row>
     <row r="9" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B9" s="22" t="n">
         <f aca="false">B8-C9</f>
@@ -10409,7 +10475,7 @@
     </row>
     <row r="10" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B10" s="22" t="n">
         <f aca="false">B9-C10</f>
@@ -10425,7 +10491,7 @@
     </row>
     <row r="11" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B11" s="22" t="n">
         <f aca="false">B10-C11</f>
@@ -10441,7 +10507,7 @@
     </row>
     <row r="12" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B12" s="22" t="n">
         <f aca="false">B11-C12</f>
@@ -10457,7 +10523,7 @@
     </row>
     <row r="13" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B13" s="22" t="n">
         <f aca="false">B12-C13</f>
@@ -10473,7 +10539,7 @@
     </row>
     <row r="14" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B14" s="22" t="n">
         <f aca="false">B13-C14</f>
@@ -10492,23 +10558,23 @@
       <c r="B15" s="22"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="E15" s="22"/>
       <c r="F15" s="22"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B16" s="29" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E16" s="29" t="s">
         <v>25</v>
@@ -10523,7 +10589,7 @@
       </c>
       <c r="B17" s="33"/>
       <c r="D17" s="35" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="E17" s="34"/>
     </row>

</xml_diff>